<commit_message>
aggiunta modifica dei punti direttamente dal sito
aggiunta aggiunta/rimozione dei punti direttamente dal sito.modificato logica della tabella,modificato display delle informazioni nella admin dashboard,aggiunto link alla casella postale
</commit_message>
<xml_diff>
--- a/instance/foglio.xlsx
+++ b/instance/foglio.xlsx
@@ -860,17 +860,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -897,10 +897,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1139,12 +1139,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1421,7 +1421,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1448,10 +1448,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -13630,7 +13630,7 @@
         <v>54</v>
       </c>
       <c r="B17" t="s" s="11">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>

</xml_diff>